<commit_message>
Add nickel blocks, laterite, and andesite alloy sheet
Introduced new blocks: raw nickel block, nickel block, laterite, and nickel-rich laterite, with corresponding loot tables and tags. Added andesite alloy sheet item and updated language files for new items and blocks. Updated gradle properties for Minecraft and mappings versions, and added related textures.
</commit_message>
<xml_diff>
--- a/dev/物品添加&修改.xlsx
+++ b/dev/物品添加&修改.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>序号</t>
   </si>
@@ -87,22 +87,13 @@
     <t>Nickel Sheet</t>
   </si>
   <si>
-    <t>crushed_raw_nickel</t>
-  </si>
-  <si>
-    <t>粉碎镍矿石</t>
-  </si>
-  <si>
-    <t>Crushed Raw Nickel</t>
-  </si>
-  <si>
     <t>raw_nickel_block</t>
   </si>
   <si>
     <t>粗镍块</t>
   </si>
   <si>
-    <t>Raw Nickel Block</t>
+    <t>Block Of Raw Nickel</t>
   </si>
   <si>
     <t>nickel_block</t>
@@ -111,7 +102,7 @@
     <t>镍块</t>
   </si>
   <si>
-    <t>Nickel Block</t>
+    <t>Block Of Nickel</t>
   </si>
   <si>
     <t>andesite_alloy_sheet</t>
@@ -121,15 +112,6 @@
   </si>
   <si>
     <t>Andesite Alloy Sheet</t>
-  </si>
-  <si>
-    <t>andesite_alloy_block</t>
-  </si>
-  <si>
-    <t>安山合金块</t>
-  </si>
-  <si>
-    <t>Andesite Alloy Block</t>
   </si>
   <si>
     <t>nickel_rich_laterite</t>
@@ -1093,10 +1075,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1255,34 +1237,6 @@
       </c>
       <c r="D10" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add aluminum and brass anvil blocks with related assets
Introduces aluminum as a new metal with ingot, nugget, sheet, and block forms, including textures and registration. Adds brass anvil, chipped brass anvil, and damaged brass anvil blocks with models, blockstates, textures, and custom damage/falling logic via mixin. Updates language files for new items and blocks, and refines mod metadata and mixin configuration.
</commit_message>
<xml_diff>
--- a/dev/物品添加&修改.xlsx
+++ b/dev/物品添加&修改.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="15015"/>
+    <workbookView windowWidth="29520" windowHeight="14055"/>
   </bookViews>
   <sheets>
     <sheet name="新增物品" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>序号</t>
   </si>
@@ -105,6 +105,15 @@
     <t>Block Of Nickel</t>
   </si>
   <si>
+    <t>nickel_nugget</t>
+  </si>
+  <si>
+    <t>镍粒</t>
+  </si>
+  <si>
+    <t>Nickel Nugget</t>
+  </si>
+  <si>
     <t>andesite_alloy_sheet</t>
   </si>
   <si>
@@ -130,6 +139,69 @@
   </si>
   <si>
     <t>Laterite</t>
+  </si>
+  <si>
+    <t>aluminum_ingot</t>
+  </si>
+  <si>
+    <t>铝锭</t>
+  </si>
+  <si>
+    <t>Aluminum Ingot</t>
+  </si>
+  <si>
+    <t>aluminum_sheet</t>
+  </si>
+  <si>
+    <t>铝板</t>
+  </si>
+  <si>
+    <t>Aluminum Sheet</t>
+  </si>
+  <si>
+    <t>aluminum_block</t>
+  </si>
+  <si>
+    <t>铝块</t>
+  </si>
+  <si>
+    <t>Block Of Aluminum</t>
+  </si>
+  <si>
+    <t>aluminum_nugget</t>
+  </si>
+  <si>
+    <t>铝粒</t>
+  </si>
+  <si>
+    <t>Aluminum Nugget</t>
+  </si>
+  <si>
+    <t>andesite_hammer</t>
+  </si>
+  <si>
+    <t>安山锤</t>
+  </si>
+  <si>
+    <t>Andesite Hammer</t>
+  </si>
+  <si>
+    <t>brass_hammer</t>
+  </si>
+  <si>
+    <t>黄铜锤</t>
+  </si>
+  <si>
+    <t>Brass Hammer</t>
+  </si>
+  <si>
+    <t>brass_anvil</t>
+  </si>
+  <si>
+    <t>黄铜砧</t>
+  </si>
+  <si>
+    <t>Brass Anvil</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1147,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1237,6 +1309,118 @@
       </c>
       <c r="D10" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>